<commit_message>
boolean extended support rollback
</commit_message>
<xml_diff>
--- a/test/FluentImporter.Demo/Files/users.xlsx
+++ b/test/FluentImporter.Demo/Files/users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haika\Desktop\Projects\Nuggets or templates\be-lib-file-importer\test\FileImporter.Demo\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HaikAsatryan\Desktop\PandaWork\Repos\Nuget repos\be-lib-fluent-importer\test\FluentImporter.Demo\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D72338-67AE-450D-A23C-AEE50F9B6969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142664BD-D402-4D3F-B106-118803EE622D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Id</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Aper</t>
+  </si>
+  <si>
+    <t>IsHuman</t>
+  </si>
+  <si>
+    <t>IsEsh</t>
   </si>
 </sst>
 </file>
@@ -355,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,7 +373,7 @@
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -377,8 +383,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -387,6 +399,12 @@
       </c>
       <c r="C2" s="1">
         <v>45316</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>